<commit_message>
Adding updated factor tracker and an older homework assignment for indices.
</commit_message>
<xml_diff>
--- a/homework/encyclopedia_quality_index/internet_encylopedic_source_quality_zach.xlsx
+++ b/homework/encyclopedia_quality_index/internet_encylopedic_source_quality_zach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zack/dat203_ccac/homework/encyclopedia_quality_index/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDD075-F2DA-D44B-B39B-49BFC9B943F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954CC81A-4C76-1045-9B01-9139FE21A70B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{8A7A157B-D150-4749-B019-79469C719DA9}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Methodology/Dictionary</t>
   </si>
   <si>
-    <t>Examining the web page and counting the number of sources cited. In order to create a more manageable number I'm dividing the number of sources by ten.</t>
-  </si>
-  <si>
     <t>Index total</t>
   </si>
   <si>
@@ -105,46 +102,49 @@
     <t># of sources cited</t>
   </si>
   <si>
-    <t>Examining the web page and counting the number of further reading links cited.</t>
-  </si>
-  <si>
     <t># ads on webpage * -1</t>
   </si>
   <si>
-    <t># sources cited / 10</t>
-  </si>
-  <si>
-    <t>All About Birds - Cornell University</t>
-  </si>
-  <si>
     <t>Tea - wiki</t>
   </si>
   <si>
-    <t>Harvard School of Public Health</t>
-  </si>
-  <si>
     <t>Hibernation - wiki</t>
   </si>
   <si>
-    <t>Discover Wildlife</t>
-  </si>
-  <si>
     <t>Electricity - wiki</t>
   </si>
   <si>
-    <t>US Energy Information Administration</t>
-  </si>
-  <si>
     <t>Water Cycle - wiki</t>
   </si>
   <si>
-    <t>USGS</t>
-  </si>
-  <si>
     <t>Mummy - wiki (redirect)</t>
   </si>
   <si>
-    <t>Smithsonian Institute</t>
+    <t>Migration of Animals - FactoMonster</t>
+  </si>
+  <si>
+    <t>Tea - FactMonster</t>
+  </si>
+  <si>
+    <t>Hibernation - FactMonster</t>
+  </si>
+  <si>
+    <t>Electricity - FactMonster</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Mummy - FactMonster</t>
+  </si>
+  <si>
+    <t># sources cited</t>
+  </si>
+  <si>
+    <t>Examining the web page and counting the number of sources cited. Either in explicit citations or written as an entry in a bibliogrpahy.</t>
+  </si>
+  <si>
+    <t>Examining the web page and counting the number of further reading links cited, if present.</t>
   </si>
 </sst>
 </file>
@@ -230,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -248,6 +248,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -567,7 +570,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -617,13 +620,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>6</v>
@@ -632,13 +635,13 @@
         <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>6</v>
@@ -649,10 +652,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="7">
-        <v>12.8</v>
+        <v>128</v>
       </c>
       <c r="D3" s="7">
         <v>0</v>
@@ -661,16 +664,16 @@
         <v>8</v>
       </c>
       <c r="F3" s="7">
-        <v>20.8</v>
+        <v>208</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H3" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I3" s="7">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="J3" s="7">
         <v>0</v>
@@ -684,10 +687,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="7">
-        <v>13.9</v>
+        <v>139</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
@@ -696,22 +699,22 @@
         <v>4</v>
       </c>
       <c r="F4" s="7">
-        <v>17.899999999999999</v>
+        <v>179</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="7">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="I4" s="7">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
       </c>
       <c r="K4" s="7">
-        <v>2.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -719,10 +722,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7">
-        <v>3.9</v>
+        <v>39</v>
       </c>
       <c r="D5" s="7">
         <v>0</v>
@@ -731,22 +734,22 @@
         <v>2</v>
       </c>
       <c r="F5" s="7">
-        <v>5.9</v>
+        <v>59</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="7">
-        <v>-25</v>
+        <v>-3</v>
       </c>
       <c r="J5" s="7">
         <v>0</v>
       </c>
       <c r="K5" s="7">
-        <v>-25</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -754,10 +757,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7">
-        <v>0.7</v>
+        <v>7</v>
       </c>
       <c r="D6" s="7">
         <v>0</v>
@@ -766,22 +769,22 @@
         <v>7</v>
       </c>
       <c r="F6" s="7">
-        <v>7.7</v>
+        <v>77</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I6" s="7">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="J6" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K6" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -789,10 +792,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7">
         <v>0</v>
@@ -801,22 +804,22 @@
         <v>1</v>
       </c>
       <c r="F7" s="7">
-        <v>4.5</v>
+        <v>45</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" s="7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
         <v>0</v>
       </c>
       <c r="J7" s="7">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K7" s="7">
-        <v>16.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -824,10 +827,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7">
-        <v>1.4</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7">
         <v>0</v>
@@ -836,22 +839,22 @@
         <v>0</v>
       </c>
       <c r="F8" s="7">
-        <v>1.4</v>
+        <v>14</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H8" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I8" s="7">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="J8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -859,76 +862,84 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="85">
+    <row r="14" spans="1:11" ht="38" customHeight="1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="102">
+    <row r="15" spans="1:11" ht="69" customHeight="1">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="102">
+    <row r="16" spans="1:11" ht="50" customHeight="1">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="51">
+    <row r="17" spans="1:6" ht="51" customHeight="1">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="34">
+    <row r="18" spans="1:6" ht="34" customHeight="1">
       <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" location=":~:text=Bird%20migration%20is%20the%20regular,Many%20species%20of%20bird%20migrate.&amp;text=It%20occurs%20mainly%20in%20the,Sea%20or%20the%20Caribbean%20Sea." xr:uid="{3C36D010-1B18-BD4A-B7BB-5AC2B4012A4D}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{FE9C19D1-8917-A143-96D7-62085113FCF1}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{B1D41763-A5A8-D047-93FE-DAE577D838B7}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{DB12EA71-C452-1847-82C1-72864F9F688E}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{3C79BE8F-ECC8-FF43-8D53-5276AB2A337B}"/>
-    <hyperlink ref="G5" r:id="rId6" xr:uid="{C0950ECF-C883-EA4D-A6B5-3A535C85F65E}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{C60C3413-1DA6-6440-88BE-9531A903C945}"/>
-    <hyperlink ref="G6" r:id="rId8" xr:uid="{A69F4068-E0B8-B94D-A6BA-7BA39C2162DA}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{96AF7C5A-EB06-3A4A-82C5-132E1C20378C}"/>
-    <hyperlink ref="G7" r:id="rId10" location="qt-science_center_objects" xr:uid="{5F6DBD7D-0067-424B-A5F0-EF18E8230A66}"/>
-    <hyperlink ref="B8" r:id="rId11" xr:uid="{094B7117-4C57-2F44-9936-391227B96CE8}"/>
-    <hyperlink ref="G8" r:id="rId12" xr:uid="{7CB78252-D0E4-C04B-835C-C4EA27663E80}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{B1D41763-A5A8-D047-93FE-DAE577D838B7}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{3C79BE8F-ECC8-FF43-8D53-5276AB2A337B}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{C60C3413-1DA6-6440-88BE-9531A903C945}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{96AF7C5A-EB06-3A4A-82C5-132E1C20378C}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{094B7117-4C57-2F44-9936-391227B96CE8}"/>
+    <hyperlink ref="G3" r:id="rId7" xr:uid="{4DB0CE34-29BA-AB41-8FA4-24B40F6573BD}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{51774595-79D1-9B42-8224-D48A1457A826}"/>
+    <hyperlink ref="G5" r:id="rId9" xr:uid="{352C880D-D08C-F847-95E0-8EBA25A31538}"/>
+    <hyperlink ref="G6" r:id="rId10" xr:uid="{722619A9-FDC5-8649-BB64-14B0EA04258F}"/>
+    <hyperlink ref="G8" r:id="rId11" xr:uid="{18C452EE-D035-ED4E-9403-CE01D0972BA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>